<commit_message>
Updated L. mandibularis barcode compliant samples
</commit_message>
<xml_diff>
--- a/Data/Myct_geneticIDs.xlsx
+++ b/Data/Myct_geneticIDs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lydia\OneDrive\Documents\GitHub\Walton-et-al-2024_FisheriesResearch-submission\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416AC195-AFD7-44C6-B99C-02B8275F31B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4322BFC4-7DDE-423C-8858-98B16D84F55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1538,11 +1538,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1900,8 +1902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="I162" sqref="I162"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C167" sqref="C167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6151,107 +6153,107 @@
         <v>335</v>
       </c>
     </row>
-    <row r="163" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A163" s="1" t="s">
+    <row r="163" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A163" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="B163" s="1" t="s">
+      <c r="B163" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C163" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E163" s="2">
+      <c r="C163" t="s">
+        <v>9</v>
+      </c>
+      <c r="E163" s="5">
         <v>44801</v>
       </c>
-      <c r="F163" s="1">
+      <c r="F163" s="4">
         <v>2022</v>
       </c>
-      <c r="G163" s="1" t="s">
+      <c r="G163" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H163" s="1" t="s">
+      <c r="H163" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="I163" s="1" t="s">
+      <c r="I163" s="4" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="164" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A164" s="1" t="s">
+    <row r="164" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A164" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B164" s="1" t="s">
+      <c r="B164" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="C164" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E164" s="2">
+      <c r="C164" t="s">
+        <v>9</v>
+      </c>
+      <c r="E164" s="5">
         <v>44801</v>
       </c>
-      <c r="F164" s="1">
+      <c r="F164" s="4">
         <v>2022</v>
       </c>
-      <c r="G164" s="1" t="s">
+      <c r="G164" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H164" s="1" t="s">
+      <c r="H164" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="I164" s="1" t="s">
+      <c r="I164" s="4" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="165" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A165" s="1" t="s">
+    <row r="165" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A165" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="B165" s="1" t="s">
+      <c r="B165" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C165" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E165" s="2">
+      <c r="C165" t="s">
+        <v>9</v>
+      </c>
+      <c r="E165" s="5">
         <v>44801</v>
       </c>
-      <c r="F165" s="1">
+      <c r="F165" s="4">
         <v>2022</v>
       </c>
-      <c r="G165" s="1" t="s">
+      <c r="G165" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H165" s="1" t="s">
+      <c r="H165" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="I165" s="1" t="s">
+      <c r="I165" s="4" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="166" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A166" s="1" t="s">
+    <row r="166" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A166" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="B166" s="1" t="s">
+      <c r="B166" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="C166" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E166" s="2">
+      <c r="C166" t="s">
+        <v>9</v>
+      </c>
+      <c r="E166" s="5">
         <v>44801</v>
       </c>
-      <c r="F166" s="1">
+      <c r="F166" s="4">
         <v>2022</v>
       </c>
-      <c r="G166" s="1" t="s">
+      <c r="G166" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H166" s="1" t="s">
+      <c r="H166" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="I166" s="1" t="s">
+      <c r="I166" s="4" t="s">
         <v>336</v>
       </c>
     </row>

</xml_diff>